<commit_message>
Update 015 FULL TABLE
</commit_message>
<xml_diff>
--- a/data/hall_of_fame.xlsx
+++ b/data/hall_of_fame.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="40">
   <si>
     <t>SEASON</t>
   </si>
@@ -47,7 +47,7 @@
     <t>DWARF</t>
   </si>
   <si>
-    <t>PHIL</t>
+    <t>FATHER TED</t>
   </si>
   <si>
     <t>2023</t>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>2022</t>
-  </si>
-  <si>
-    <t>FATHER TED</t>
   </si>
   <si>
     <t>2021</t>
@@ -134,7 +131,7 @@
     <t>TEL</t>
   </si>
   <si>
-    <t>DAVE M</t>
+    <t>DOGGER</t>
   </si>
 </sst>
 </file>
@@ -25697,7 +25694,7 @@
         <v>17</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C8" s="4">
         <v>35.0</v>
@@ -25736,7 +25733,7 @@
     </row>
     <row r="9">
       <c r="A9" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>13</v>
@@ -25865,7 +25862,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="4">
         <v>34.0</v>
@@ -25904,7 +25901,7 @@
     </row>
     <row r="13">
       <c r="A13" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>13</v>
@@ -26033,7 +26030,7 @@
         <v>17</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="C16" s="4">
         <v>20.0</v>
@@ -26072,7 +26069,7 @@
     </row>
     <row r="17">
       <c r="A17" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>13</v>
@@ -26201,7 +26198,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="4">
         <v>40.0</v>
@@ -26240,7 +26237,7 @@
     </row>
     <row r="21">
       <c r="A21" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>13</v>
@@ -26327,7 +26324,7 @@
         <v>15</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C23" s="5">
         <v>32.0</v>
@@ -26369,7 +26366,7 @@
         <v>17</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C24" s="5">
         <v>41.0</v>
@@ -26408,7 +26405,7 @@
     </row>
     <row r="25">
       <c r="A25" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>13</v>
@@ -26495,7 +26492,7 @@
         <v>15</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" s="5">
         <v>33.0</v>
@@ -26537,7 +26534,7 @@
         <v>17</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" s="5">
         <v>30.0</v>
@@ -26576,7 +26573,7 @@
     </row>
     <row r="29">
       <c r="A29" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>13</v>
@@ -26705,7 +26702,7 @@
         <v>17</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" s="5">
         <v>40.0</v>
@@ -26744,7 +26741,7 @@
     </row>
     <row r="33">
       <c r="A33" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>13</v>
@@ -26831,7 +26828,7 @@
         <v>15</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C35" s="6">
         <v>45.0</v>
@@ -26873,7 +26870,7 @@
         <v>17</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36" s="6">
         <v>39.0</v>
@@ -26912,7 +26909,7 @@
     </row>
     <row r="37">
       <c r="A37" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>13</v>
@@ -26999,7 +26996,7 @@
         <v>15</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C39" s="9">
         <v>37.0</v>
@@ -27080,7 +27077,7 @@
     </row>
     <row r="41">
       <c r="A41" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>13</v>
@@ -27209,7 +27206,7 @@
         <v>17</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C44" s="5">
         <v>42.0</v>
@@ -27248,7 +27245,7 @@
     </row>
     <row r="45">
       <c r="A45" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>13</v>
@@ -27335,7 +27332,7 @@
         <v>15</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C47" s="5">
         <v>36.0</v>
@@ -27377,7 +27374,7 @@
         <v>17</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C48" s="5">
         <v>32.0</v>

</xml_diff>